<commit_message>
🤖 自动更新价格数据 2025-11-22 03:29:16
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -468,6 +468,22 @@
         <v>1112</v>
       </c>
       <c r="D2" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D3" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-23 04:02:51
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -484,6 +484,22 @@
         <v>1112</v>
       </c>
       <c r="D3" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D4" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-24 04:02:40
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -500,6 +500,22 @@
         <v>1112</v>
       </c>
       <c r="D4" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D5" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-25 03:42:58
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -516,6 +516,22 @@
         <v>1112</v>
       </c>
       <c r="D5" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D6" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-26 03:43:09
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -532,6 +532,22 @@
         <v>1112</v>
       </c>
       <c r="D6" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D7" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-27 03:39:14
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,16 +538,32 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="B8" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D8" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-28 03:39:03
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,16 +554,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="B9" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D9" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-29 03:39:43
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,16 +570,32 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="B10" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D10" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-11-30 04:03:42
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,16 +586,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="B11" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D11" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-01 04:37:26
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,16 +602,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="B12" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D12" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-02 03:56:51
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,16 +618,32 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D12" t="n">
+      <c r="B13" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D13" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-03 03:55:10
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,16 +634,32 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D13" t="n">
+      <c r="B14" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D14" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-04 03:56:57
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,16 +650,32 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D14" t="n">
+      <c r="B15" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D15" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-05 03:55:51
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,16 +666,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D15" t="n">
+      <c r="B16" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D16" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-06 03:35:52
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,16 +682,32 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D16" t="n">
+      <c r="B17" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D17" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-07 04:03:05
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,16 +698,32 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D17" t="n">
+      <c r="B18" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D18" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-08 04:00:52
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,16 +714,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D18" t="n">
+      <c r="B19" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D19" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-09 03:54:50
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,16 +730,32 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D19" t="n">
+      <c r="B20" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D20" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-10 04:01:08
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,16 +746,32 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B20" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D20" t="n">
+      <c r="B21" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D21" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-11 04:03:09
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,16 +762,32 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D21" t="n">
+      <c r="B22" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D22" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-12 04:02:35
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,16 +778,32 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D22" t="n">
+      <c r="B23" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D23" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-13 03:52:43
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,16 +794,32 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D23" t="n">
+      <c r="B24" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D24" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-14 04:07:23
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,16 +810,32 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B24" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D24" t="n">
+      <c r="B25" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D25" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-15 04:12:53
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,16 +826,32 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B25" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D25" t="n">
+      <c r="B26" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D26" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-16 04:03:49
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,16 +842,32 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D26" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B26" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D26" t="n">
+      <c r="B27" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D27" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-17 03:59:59
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,16 +858,32 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D27" t="n">
+      <c r="B28" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D28" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-18 04:01:09
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,16 +874,32 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B28" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D28" t="n">
+      <c r="B29" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D29" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-19 04:03:17
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,16 +890,32 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D29" t="n">
+      <c r="B30" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D30" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-20 03:52:21
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,16 +906,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B30" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D30" t="n">
+      <c r="B31" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D31" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-21 04:07:46
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,16 +922,32 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B31" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D31" t="n">
+      <c r="B32" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D32" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-22 04:12:56
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,16 +938,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B32" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D32" t="n">
+      <c r="B33" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D33" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-23 02:48:22
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,16 +954,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B33" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D33" t="n">
+      <c r="B34" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D34" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-24 02:46:08
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,16 +970,32 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D34" t="n">
+      <c r="B35" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D35" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-25 02:48:59
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,16 +986,32 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B35" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D35" t="n">
+      <c r="B36" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D36" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-26 02:47:17
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,16 +1002,32 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B36" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D36" t="n">
+      <c r="B37" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D37" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-27 02:44:20
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,16 +1018,32 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B37" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D37" t="n">
+      <c r="B38" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D38" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-28 03:00:35
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,16 +1034,32 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B38" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D38" t="n">
+      <c r="B39" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D39" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-29 03:00:35
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,16 +1050,32 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B39" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D39" t="n">
+      <c r="B40" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D40" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-30 02:49:53
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,16 +1066,32 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D40" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B40" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D40" t="n">
+      <c r="B41" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D41" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2025-12-31 02:49:12
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,16 +1082,32 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D41" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B41" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C41" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D41" t="n">
+      <c r="B42" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D42" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-01 03:01:29
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,16 +1098,32 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B42" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C42" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D42" t="n">
+      <c r="B43" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D43" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-02 02:52:28
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,16 +1114,32 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D43" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B43" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C43" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D43" t="n">
+      <c r="B44" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D44" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-03 02:43:45
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,16 +1130,32 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D44" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B44" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C44" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D44" t="n">
+      <c r="B45" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D45" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-04 03:03:14
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,16 +1146,32 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B45" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C45" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D45" t="n">
+      <c r="B46" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D46" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-05 03:05:18
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,16 +1162,32 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B46" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C46" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D46" t="n">
+      <c r="B47" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D47" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-06 02:51:38
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,16 +1178,32 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D47" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B47" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C47" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D47" t="n">
+      <c r="B48" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D48" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-07 02:51:52
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,16 +1194,32 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D48" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B48" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C48" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D48" t="n">
+      <c r="B49" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D49" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-08 02:51:21
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,16 +1210,32 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D49" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B49" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C49" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D49" t="n">
+      <c r="B50" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D50" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-09 02:52:21
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,16 +1226,32 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B50" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C50" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D50" t="n">
+      <c r="B51" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D51" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-10 02:45:52
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,16 +1242,32 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B51" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C51" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D51" t="n">
+      <c r="B52" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D52" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-11 03:02:32
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,16 +1258,32 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D52" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B52" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C52" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D52" t="n">
+      <c r="B53" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D53" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-12 03:00:13
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,16 +1274,32 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D53" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B53" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C53" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D53" t="n">
+      <c r="B54" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D54" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-13 02:50:04
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,16 +1290,32 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B54" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C54" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D54" t="n">
+      <c r="B55" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D55" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-14 02:58:25
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,16 +1306,32 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B55" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C55" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D55" t="n">
+      <c r="B56" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D56" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-15 02:52:12
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,16 +1322,32 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B56" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C56" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D56" t="n">
+      <c r="B57" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D57" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-16 02:53:27
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,16 +1338,32 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D57" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B57" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C57" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D57" t="n">
+      <c r="B58" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D58" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-17 02:44:24
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1338,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,16 +1354,32 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B58" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C58" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D58" t="n">
+      <c r="B59" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D59" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-18 03:00:58
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1338,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,7 +1354,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1370,16 +1370,32 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D59" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B59" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C59" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D59" t="n">
+      <c r="B60" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D60" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-19 03:00:54
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1338,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,7 +1354,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1370,7 +1370,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1386,16 +1386,32 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B60" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C60" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D60" t="n">
+      <c r="B61" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D61" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-20 02:54:45
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1338,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,7 +1354,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1370,7 +1370,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1386,7 +1386,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1402,16 +1402,32 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D61" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B61" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C61" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D61" t="n">
+      <c r="B62" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D62" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-21 02:53:51
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +474,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +490,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +522,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +538,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +554,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +570,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +586,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +602,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +618,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +634,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +650,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +666,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +682,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +698,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +714,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +730,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +746,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +762,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +778,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +810,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +826,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +858,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +874,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +890,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +906,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +922,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +938,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +954,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +970,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +1002,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1018,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1034,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1050,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1066,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1082,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1098,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1114,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1130,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1146,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1162,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1178,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1194,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1210,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1338,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,7 +1354,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1370,7 +1370,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1386,7 +1386,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1402,7 +1402,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1418,16 +1418,32 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D62" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B62" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C62" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D62" t="n">
+      <c r="B63" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D63" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-22 02:59:12
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,22 +422,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>日期</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>铁矿石(元/吨)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>焦煤(元/吨)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>H型钢材(元/吨)</t>
         </is>
@@ -458,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -474,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -490,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -506,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -522,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -538,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -554,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -570,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -586,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -602,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -618,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -634,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -650,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -666,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -682,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -698,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -714,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -730,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -746,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -762,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -778,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -794,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -826,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -842,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -858,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -874,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -890,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -906,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -922,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -938,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -954,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -970,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -986,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1002,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1018,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1034,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1050,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1066,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1082,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1098,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1114,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1130,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1146,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1162,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1178,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1194,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1210,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1226,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1370,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1386,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1402,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1418,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1434,16 +1422,32 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D63" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B63" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C63" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D63" t="n">
+      <c r="B64" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D64" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-23 02:54:18
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,16 +1438,32 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D64" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B64" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C64" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D64" t="n">
+      <c r="B65" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D65" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-24 02:48:37
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,16 +1454,32 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D65" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B65" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C65" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D65" t="n">
+      <c r="B66" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D66" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-25 03:06:02
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,16 +1470,32 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D66" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B66" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C66" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D66" t="n">
+      <c r="B67" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D67" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-26 03:07:43
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,16 +1486,32 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D67" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B67" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C67" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D67" t="n">
+      <c r="B68" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D68" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-27 02:59:56
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,16 +1502,32 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D68" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B68" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C68" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D68" t="n">
+      <c r="B69" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D69" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-28 02:56:52
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,16 +1518,32 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D69" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B69" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C69" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D69" t="n">
+      <c r="B70" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D70" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-29 03:19:19
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,16 +1534,32 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D70" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B70" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C70" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D70" t="n">
+      <c r="B71" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D71" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-30 03:21:23
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,16 +1550,32 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D71" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B71" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C71" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D71" t="n">
+      <c r="B72" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D72" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-01-31 03:13:09
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,16 +1566,32 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D72" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B72" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C72" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D72" t="n">
+      <c r="B73" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D73" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-01 03:43:17
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,16 +1582,32 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D73" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B73" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C73" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D73" t="n">
+      <c r="B74" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D74" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-02 03:34:46
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,16 +1598,32 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D74" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B74" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C74" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D74" t="n">
+      <c r="B75" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D75" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-03 03:28:37
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,16 +1614,32 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D75" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B75" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C75" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D75" t="n">
+      <c r="B76" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D76" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-04 03:25:48
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,16 +1630,32 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D76" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B76" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C76" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D76" t="n">
+      <c r="B77" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D77" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-05 03:26:53
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,16 +1646,32 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C77" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D77" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B77" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C77" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D77" t="n">
+      <c r="B78" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D78" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-06 03:25:50
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,16 +1662,32 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C78" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D78" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B78" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C78" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D78" t="n">
+      <c r="B79" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D79" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-07 03:15:53
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,16 +1678,32 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C79" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D79" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B79" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C79" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D79" t="n">
+      <c r="B80" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D80" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-08 03:48:48
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,16 +1694,32 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D80" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B80" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C80" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D80" t="n">
+      <c r="B81" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D81" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-09 03:36:57
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,16 +1710,32 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D81" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B81" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C81" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D81" t="n">
+      <c r="B82" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D82" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-10 03:45:13
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,16 +1726,32 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D82" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B82" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C82" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D82" t="n">
+      <c r="B83" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D83" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-11 03:42:23
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,16 +1742,32 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D83" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B83" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C83" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D83" t="n">
+      <c r="B84" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D84" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-12 03:36:40
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,16 +1758,32 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C84" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D84" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B84" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C84" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D84" t="n">
+      <c r="B85" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D85" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-13 03:35:17
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,16 +1774,32 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D85" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B85" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C85" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D85" t="n">
+      <c r="B86" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D86" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-14 03:22:10
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,16 +1790,32 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D86" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B86" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C86" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D86" t="n">
+      <c r="B87" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D87" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-15 03:36:14
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,16 +1806,32 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D87" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B87" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C87" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D87" t="n">
+      <c r="B88" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D88" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-16 03:35:01
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,16 +1822,32 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D88" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B88" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C88" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D88" t="n">
+      <c r="B89" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D89" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-17 03:29:38
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,7 +1822,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1838,16 +1838,32 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D89" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B89" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C89" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D89" t="n">
+      <c r="B90" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D90" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-18 03:32:26
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,7 +1822,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1838,7 +1838,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1854,16 +1854,32 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D90" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B90" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C90" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D90" t="n">
+      <c r="B91" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D91" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-19 03:31:19
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,7 +1822,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1838,7 +1838,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1854,7 +1854,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1870,16 +1870,32 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D91" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B91" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C91" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D91" t="n">
+      <c r="B92" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D92" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-20 03:26:25
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,7 +1822,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1838,7 +1838,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1854,7 +1854,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1870,7 +1870,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -1886,16 +1886,32 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D92" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B92" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C92" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D92" t="n">
+      <c r="B93" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D93" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-21 03:14:25
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-21</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,7 +1822,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1838,7 +1838,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1854,7 +1854,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1870,7 +1870,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -1886,7 +1886,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -1902,16 +1902,32 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D93" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B93" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C93" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D93" t="n">
+      <c r="B94" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D94" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>

<commit_message>
🤖 自动更新价格数据 2026-02-22 03:30:45
</commit_message>
<xml_diff>
--- a/商品价格数据.xlsx
+++ b/商品价格数据.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2026-02-21</t>
+          <t>2026-02-22</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -462,7 +462,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2026-02-20</t>
+          <t>2026-02-21</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -478,7 +478,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2026-02-19</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -494,7 +494,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-19</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -510,7 +510,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2026-02-17</t>
+          <t>2026-02-18</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -526,7 +526,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2026-02-16</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -542,7 +542,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2026-02-15</t>
+          <t>2026-02-16</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -558,7 +558,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2026-02-14</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -574,7 +574,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2026-02-13</t>
+          <t>2026-02-14</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -590,7 +590,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-12</t>
+          <t>2026-02-13</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -606,7 +606,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2026-02-11</t>
+          <t>2026-02-12</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -622,7 +622,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2026-02-10</t>
+          <t>2026-02-11</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -638,7 +638,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2026-02-09</t>
+          <t>2026-02-10</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -654,7 +654,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2026-02-08</t>
+          <t>2026-02-09</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -670,7 +670,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2026-02-07</t>
+          <t>2026-02-08</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -686,7 +686,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2026-02-06</t>
+          <t>2026-02-07</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -702,7 +702,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2026-02-05</t>
+          <t>2026-02-06</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -718,7 +718,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2026-02-04</t>
+          <t>2026-02-05</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -734,7 +734,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2026-02-03</t>
+          <t>2026-02-04</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -750,7 +750,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2026-02-02</t>
+          <t>2026-02-03</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -766,7 +766,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2026-02-01</t>
+          <t>2026-02-02</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -782,7 +782,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-31</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -798,7 +798,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-31</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -814,7 +814,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-01-29</t>
+          <t>2026-01-30</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -830,7 +830,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-01-28</t>
+          <t>2026-01-29</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -846,7 +846,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-01-27</t>
+          <t>2026-01-28</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -862,7 +862,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-01-26</t>
+          <t>2026-01-27</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -878,7 +878,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-26</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -894,7 +894,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-01-24</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -910,7 +910,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-24</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -926,7 +926,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-01-22</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -942,7 +942,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-01-21</t>
+          <t>2026-01-22</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -958,7 +958,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-01-20</t>
+          <t>2026-01-21</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -974,7 +974,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2026-01-19</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -990,7 +990,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2026-01-18</t>
+          <t>2026-01-19</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1006,7 +1006,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2026-01-17</t>
+          <t>2026-01-18</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1022,7 +1022,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2026-01-16</t>
+          <t>2026-01-17</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1038,7 +1038,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2026-01-15</t>
+          <t>2026-01-16</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1054,7 +1054,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2026-01-14</t>
+          <t>2026-01-15</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1070,7 +1070,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2026-01-13</t>
+          <t>2026-01-14</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1086,7 +1086,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2026-01-12</t>
+          <t>2026-01-13</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -1102,7 +1102,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-12</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1118,7 +1118,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2026-01-10</t>
+          <t>2026-01-11</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1134,7 +1134,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2026-01-09</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1150,7 +1150,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2026-01-08</t>
+          <t>2026-01-09</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1166,7 +1166,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2026-01-07</t>
+          <t>2026-01-08</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1182,7 +1182,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2026-01-06</t>
+          <t>2026-01-07</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1198,7 +1198,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2026-01-05</t>
+          <t>2026-01-06</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1214,7 +1214,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2026-01-04</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1230,7 +1230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2026-01-03</t>
+          <t>2026-01-04</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1246,7 +1246,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2026-01-02</t>
+          <t>2026-01-03</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1262,7 +1262,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2026-01-01</t>
+          <t>2026-01-02</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1278,7 +1278,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1294,7 +1294,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-31</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1310,7 +1310,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2025-12-29</t>
+          <t>2025-12-30</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1326,7 +1326,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2025-12-28</t>
+          <t>2025-12-29</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1342,7 +1342,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2025-12-27</t>
+          <t>2025-12-28</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1358,7 +1358,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2025-12-26</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1374,7 +1374,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2025-12-25</t>
+          <t>2025-12-26</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1390,7 +1390,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2025-12-24</t>
+          <t>2025-12-25</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1406,7 +1406,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-24</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1422,7 +1422,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2025-12-22</t>
+          <t>2025-12-23</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1438,7 +1438,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2025-12-21</t>
+          <t>2025-12-22</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1454,7 +1454,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2025-12-20</t>
+          <t>2025-12-21</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1470,7 +1470,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2025-12-19</t>
+          <t>2025-12-20</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1486,7 +1486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1502,7 +1502,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2025-12-17</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -1518,7 +1518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-17</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1534,7 +1534,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1550,7 +1550,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2025-12-14</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1566,7 +1566,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2025-12-13</t>
+          <t>2025-12-14</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -1582,7 +1582,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2025-12-12</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1598,7 +1598,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2025-12-11</t>
+          <t>2025-12-12</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1614,7 +1614,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2025-12-10</t>
+          <t>2025-12-11</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1630,7 +1630,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2025-12-09</t>
+          <t>2025-12-10</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1646,7 +1646,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-09</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1662,7 +1662,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2025-12-07</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1678,7 +1678,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2025-12-06</t>
+          <t>2025-12-07</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1694,7 +1694,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2025-12-05</t>
+          <t>2025-12-06</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1710,7 +1710,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1726,7 +1726,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-04</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1742,7 +1742,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1758,7 +1758,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1774,7 +1774,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1790,7 +1790,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-11-30</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1806,7 +1806,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1822,7 +1822,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2025-11-27</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1838,7 +1838,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2025-11-26</t>
+          <t>2025-11-27</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1854,7 +1854,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2025-11-25</t>
+          <t>2025-11-26</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1870,7 +1870,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2025-11-24</t>
+          <t>2025-11-25</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -1886,7 +1886,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2025-11-23</t>
+          <t>2025-11-24</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -1902,7 +1902,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-23</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -1918,16 +1918,32 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D94" t="n">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>2025-11-21</t>
         </is>
       </c>
-      <c r="B94" t="n">
-        <v>783.5</v>
-      </c>
-      <c r="C94" t="n">
-        <v>1112</v>
-      </c>
-      <c r="D94" t="n">
+      <c r="B95" t="n">
+        <v>783.5</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D95" t="n">
         <v>3610</v>
       </c>
     </row>

</xml_diff>